<commit_message>
Actualizado relatorio e schema participants.
</commit_message>
<xml_diff>
--- a/Relatório Projecto Final/Schemas/Participants/participantsSchema.xlsx
+++ b/Relatório Projecto Final/Schemas/Participants/participantsSchema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silvia\ISEL\Repositorio Local\PDM\Relatório Projecto Final\Schemas\Participants\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lima\ISEL\Ano 3\Semestre 5\PDM\repositorio\Relatório Projecto Final\Schemas\Participants\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -92,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -104,21 +104,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -236,17 +221,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -254,27 +231,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -986,7 +970,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,130 +984,137 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="7"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="8"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="I4" s="19"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="K5" s="2" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="9"/>
+      <c r="K5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="16"/>
-      <c r="M5" s="3"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="11"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="D8" s="1" t="s">
+      <c r="B8" s="11"/>
+      <c r="D8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="17" t="s">
+      <c r="E8" s="15"/>
+      <c r="F8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="17"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
       <c r="E11" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G12" s="7"/>
-      <c r="H12" s="2" t="s">
+      <c r="G12" s="4"/>
+      <c r="H12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="8"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="11"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="11"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="13"/>
+      <c r="K16" s="12"/>
     </row>
     <row r="17" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="3"/>
+      <c r="J18" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A11:C11"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="K5:M5"/>
@@ -1132,13 +1123,6 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H7:J7"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>